<commit_message>
add example values to metabolights templates
</commit_message>
<xml_diff>
--- a/templates/dataplant/MetaboLights/MetaboLights_-_Chromatography.xlsx
+++ b/templates/dataplant/MetaboLights/MetaboLights_-_Chromatography.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="82">
   <si>
     <t>TEMPLATE</t>
   </si>
@@ -32,7 +32,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.1</t>
+    <t>1.0.2</t>
   </si>
   <si>
     <t>Description</t>
@@ -231,6 +231,33 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>Gas Chromatography</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C30014</t>
+  </si>
+  <si>
+    <t>2 ml ethyl acetate</t>
+  </si>
+  <si>
+    <t>trimethylsilyl derivatisation</t>
+  </si>
+  <si>
+    <t>CHMO</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CHMO_0002758</t>
+  </si>
+  <si>
+    <t>Shimadzu GCMS-QP2010 Ultra</t>
+  </si>
+  <si>
+    <t>Zebron ZB-AAA GC(10 m x 0.25 mm; Phenomenex)</t>
+  </si>
+  <si>
+    <t>medium polarity</t>
   </si>
 </sst>
 </file>
@@ -934,19 +961,19 @@
         <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E2" t="s">
         <v>72</v>
       </c>
       <c r="F2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="G2" t="s">
         <v>72</v>
@@ -955,16 +982,16 @@
         <v>72</v>
       </c>
       <c r="I2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="J2" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="K2" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="L2" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="M2" t="s">
         <v>72</v>
@@ -973,7 +1000,7 @@
         <v>72</v>
       </c>
       <c r="O2" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="P2" t="s">
         <v>72</v>
@@ -982,7 +1009,7 @@
         <v>72</v>
       </c>
       <c r="R2" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="S2" t="s">
         <v>72</v>

</xml_diff>

<commit_message>
update example terms for metabolights
</commit_message>
<xml_diff>
--- a/templates/dataplant/MetaboLights/MetaboLights_-_Chromatography.xlsx
+++ b/templates/dataplant/MetaboLights/MetaboLights_-_Chromatography.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="83">
   <si>
     <t>TEMPLATE</t>
   </si>
@@ -258,6 +258,9 @@
   </si>
   <si>
     <t>medium polarity</t>
+  </si>
+  <si>
+    <t>13C</t>
   </si>
 </sst>
 </file>
@@ -1018,7 +1021,7 @@
         <v>72</v>
       </c>
       <c r="U2" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="V2" t="s">
         <v>72</v>

</xml_diff>